<commit_message>
Added "empty_cols" to NGIT,edited NGIT placements
</commit_message>
<xml_diff>
--- a/Files/college_info/all_colleges/NGIT/NGIT_placements.xlsx
+++ b/Files/college_info/all_colleges/NGIT/NGIT_placements.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mugdha\Desktop\python project\self\NGIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mugdha\Desktop\python project\github\python_project-dataset\Files\college_info\all_colleges\NGIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F210304-487D-4962-8672-F5ED683EF1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBA4AC8-BBCC-4BCD-AA70-7266814C120C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$D$80</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
   <si>
     <t>COMPANY</t>
   </si>
@@ -36,18 +39,12 @@
     <t>Adobe</t>
   </si>
   <si>
-    <t>SILICON LABS</t>
-  </si>
-  <si>
     <t>EXPERIAN</t>
   </si>
   <si>
     <t>DARWINBOX</t>
   </si>
   <si>
-    <t>NCR</t>
-  </si>
-  <si>
     <t>SALESFORCE</t>
   </si>
   <si>
@@ -57,15 +54,9 @@
     <t>CyberArk</t>
   </si>
   <si>
-    <t>ZENSAR</t>
-  </si>
-  <si>
     <t>DBS</t>
   </si>
   <si>
-    <t>INFOR</t>
-  </si>
-  <si>
     <t>Infosys (PP)</t>
   </si>
   <si>
@@ -96,9 +87,6 @@
     <t>LENSKART</t>
   </si>
   <si>
-    <t>Zemoso Labs</t>
-  </si>
-  <si>
     <t>Veeva Systems</t>
   </si>
   <si>
@@ -117,9 +105,6 @@
     <t>Infosys (DSE)</t>
   </si>
   <si>
-    <t>VIRTUSA</t>
-  </si>
-  <si>
     <t>MODAK</t>
   </si>
   <si>
@@ -253,13 +238,49 @@
   </si>
   <si>
     <t>OFFERS</t>
+  </si>
+  <si>
+    <t>INFOR_8.5</t>
+  </si>
+  <si>
+    <t>INFOR_6</t>
+  </si>
+  <si>
+    <t>NCR_14</t>
+  </si>
+  <si>
+    <t>NCR_10</t>
+  </si>
+  <si>
+    <t>SILICON LABS_21.5</t>
+  </si>
+  <si>
+    <t>SILICON LABS_10</t>
+  </si>
+  <si>
+    <t>VIRTUSA_6</t>
+  </si>
+  <si>
+    <t>VIRTUSA_4.5</t>
+  </si>
+  <si>
+    <t>Zemoso Labs_7.5</t>
+  </si>
+  <si>
+    <t>Zemoso Labs_6.8</t>
+  </si>
+  <si>
+    <t>ZENSAR_9</t>
+  </si>
+  <si>
+    <t>ZENSAR_4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +300,14 @@
       <color rgb="FF252525"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -322,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -330,6 +359,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,36 +641,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>73</v>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -653,7 +683,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -667,11 +697,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="C4" s="2">
         <v>21.5</v>
@@ -681,11 +711,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2">
         <v>16</v>
@@ -695,11 +725,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2">
         <v>15.5</v>
@@ -709,11 +739,11 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2">
         <v>14</v>
@@ -723,11 +753,11 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2">
         <v>13</v>
@@ -737,11 +767,11 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2">
         <v>12</v>
@@ -751,39 +781,39 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2">
         <v>10</v>
       </c>
       <c r="D10" s="2">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="C11" s="2">
         <v>10</v>
       </c>
       <c r="D11" s="2">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="C12" s="2">
         <v>10</v>
@@ -793,39 +823,39 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
         <v>9</v>
       </c>
       <c r="D13" s="2">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="C14" s="2">
         <v>9</v>
       </c>
       <c r="D14" s="2">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C15" s="2">
         <v>8.5</v>
@@ -835,11 +865,11 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2">
         <v>8</v>
@@ -849,53 +879,53 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2">
         <v>8</v>
       </c>
       <c r="D17" s="2">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C18" s="2">
         <v>8</v>
       </c>
       <c r="D18" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="2">
         <v>8</v>
       </c>
       <c r="D19" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C20" s="2">
         <v>8</v>
@@ -905,319 +935,319 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" s="2">
         <v>8</v>
       </c>
       <c r="D21" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C22" s="2">
         <v>8</v>
       </c>
       <c r="D22" s="2">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C23" s="2">
         <v>8</v>
       </c>
       <c r="D23" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C24" s="2">
+        <v>7.82</v>
+      </c>
+      <c r="D24" s="2">
         <v>8</v>
       </c>
-      <c r="D24" s="2">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="D25" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="2">
-        <v>7.82</v>
-      </c>
-      <c r="D25" s="2">
-        <v>8</v>
-      </c>
-    </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="C26" s="2">
         <v>7.5</v>
       </c>
       <c r="D26" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C27" s="2">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="D27" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C28" s="2">
         <v>7</v>
       </c>
       <c r="D28" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C29" s="2">
         <v>7</v>
       </c>
       <c r="D29" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C30" s="2">
         <v>7</v>
       </c>
       <c r="D30" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="C31" s="2">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="D31" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="2">
-        <v>6.8</v>
+        <v>6.75</v>
       </c>
       <c r="D32" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C33" s="2">
-        <v>6.75</v>
+        <v>6.25</v>
       </c>
       <c r="D33" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="2">
         <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="2">
-        <v>6.25</v>
       </c>
       <c r="D34" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="4">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C35" s="2">
         <v>6</v>
       </c>
       <c r="D35" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="4">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C36" s="2">
         <v>6</v>
       </c>
       <c r="D36" s="2">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="A37" s="4">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="C37" s="2">
         <v>6</v>
       </c>
       <c r="D37" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="A38" s="4">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C38" s="2">
         <v>6</v>
       </c>
       <c r="D38" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+      <c r="A39" s="4">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C39" s="2">
         <v>6</v>
       </c>
       <c r="D39" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" s="2">
         <v>6</v>
       </c>
       <c r="D40" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+      <c r="A41" s="4">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C41" s="2">
         <v>6</v>
       </c>
       <c r="D41" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="4">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C42" s="2">
         <v>6</v>
       </c>
       <c r="D42" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="A43" s="4">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C43" s="2">
         <v>6</v>
@@ -1227,11 +1257,11 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+      <c r="A44" s="4">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C44" s="2">
         <v>6</v>
@@ -1241,11 +1271,11 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+      <c r="A45" s="4">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C45" s="2">
         <v>6</v>
@@ -1254,418 +1284,418 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="C46" s="2">
         <v>6</v>
       </c>
       <c r="D46" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="A47" s="4">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C47" s="2">
-        <v>6</v>
+        <v>5.7</v>
       </c>
       <c r="D47" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="A48" s="4">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C48" s="2">
-        <v>5.7</v>
+        <v>5.5</v>
       </c>
       <c r="D48" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C49" s="2">
         <v>5.5</v>
       </c>
       <c r="D49" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C50" s="2">
         <v>5.5</v>
       </c>
       <c r="D50" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C51" s="2">
-        <v>5.5</v>
+        <v>5.4</v>
       </c>
       <c r="D51" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C52" s="2">
-        <v>5.4</v>
+        <v>5</v>
       </c>
       <c r="D52" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="A53" s="4">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C53" s="2">
         <v>5</v>
       </c>
       <c r="D53" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
+      <c r="A54" s="4">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C54" s="2">
         <v>5</v>
       </c>
       <c r="D54" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+      <c r="A55" s="4">
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C55" s="2">
         <v>5</v>
       </c>
       <c r="D55" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+      <c r="A56" s="4">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C56" s="2">
         <v>5</v>
       </c>
       <c r="D56" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+      <c r="A57" s="4">
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" s="2">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C58" s="2">
+        <v>4.72</v>
+      </c>
+      <c r="D58" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C59" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C57" s="2">
-        <v>5</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
-        <v>57</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C58" s="2">
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="D58" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
-        <v>58</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C59" s="2">
-        <v>4.72</v>
-      </c>
-      <c r="D59" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
-        <v>59</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="C60" s="2">
         <v>4.5</v>
       </c>
       <c r="D60" s="2">
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
+      <c r="A61" s="4">
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C61" s="2">
         <v>4.5</v>
       </c>
       <c r="D61" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="C62" s="2">
         <v>4.5</v>
       </c>
       <c r="D62" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C63" s="2">
         <v>4.5</v>
       </c>
       <c r="D63" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
+      <c r="A64" s="4">
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C64" s="2">
         <v>4.5</v>
       </c>
       <c r="D64" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+      <c r="A65" s="4">
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C65" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>65</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C65" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="D65" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
-        <v>65</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="C66" s="2">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="D66" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="A67" s="4">
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C67" s="2">
         <v>4</v>
       </c>
       <c r="D67" s="2">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+      <c r="A68" s="4">
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C68" s="2">
         <v>4</v>
       </c>
       <c r="D68" s="2">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
+      <c r="A69" s="4">
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C69" s="2">
         <v>4</v>
       </c>
       <c r="D69" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
+      <c r="A70" s="4">
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C70" s="2">
         <v>4</v>
       </c>
       <c r="D70" s="2">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
+      <c r="A71" s="4">
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C71" s="2">
         <v>4</v>
       </c>
       <c r="D71" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
+      <c r="A72" s="4">
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C72" s="2">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="D72" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
+      <c r="A73" s="4">
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C73" s="2">
         <v>3.6</v>
       </c>
       <c r="D73" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
+      <c r="A74" s="4">
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C74" s="2">
         <v>3.6</v>
       </c>
       <c r="D74" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
+      <c r="A75" s="4">
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C75" s="2">
         <v>3.6</v>
@@ -1675,90 +1705,82 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
+      <c r="A76" s="4">
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C76" s="2">
         <v>3.6</v>
       </c>
       <c r="D76" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C77" s="2">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="D77" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C78" s="2">
         <v>3.5</v>
       </c>
       <c r="D78" s="2">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
+      <c r="A79" s="4">
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C79" s="2">
         <v>3.5</v>
       </c>
       <c r="D79" s="2">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
+      <c r="A80" s="4">
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C80" s="2">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="D80" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
-        <v>80</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C81" s="2">
-        <v>3</v>
-      </c>
-      <c r="D81" s="2">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="B1:D80" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D80">
+      <sortCondition descending="1" ref="C1:C80"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>